<commit_message>
bill banana and avocado
</commit_message>
<xml_diff>
--- a/data/B/experiment2/avocado covariate.xlsx
+++ b/data/B/experiment2/avocado covariate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koohong\Documents\MIDS\MIDS241\mids-w241-fa2020-fp\data\B\experiment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917FFE34-787F-4C34-9C16-4BBEAA6993AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754621A6-26C0-4B79-B8F4-68E93950AF15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9C195F2C-2221-4830-B3B1-52CA74A48640}"/>
   </bookViews>
@@ -401,7 +401,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>